<commit_message>
moving to signals (WIP).
</commit_message>
<xml_diff>
--- a/paperwork/relations.xlsx
+++ b/paperwork/relations.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dehmer/Development/bmlv.gv.at/3c041181/paperwork/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2A165B59-7FA3-954A-A5AF-1E7B7214EE9E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3BD8210E-9532-3C4E-B512-A69892D52BFE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="720" windowWidth="29400" windowHeight="18400" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -575,8 +575,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="C4:AJ33"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B4" zoomScale="111" zoomScaleNormal="75" workbookViewId="0">
-      <selection activeCell="C19" sqref="C19"/>
+    <sheetView tabSelected="1" topLeftCell="C4" zoomScale="150" zoomScaleNormal="75" workbookViewId="0">
+      <selection activeCell="AG18" sqref="AG18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="17" x14ac:dyDescent="0.25"/>

</xml_diff>